<commit_message>
Translate newdir/test.xlsx in es
100% translated source file: 'newdir/test.xlsx'
on 'es'.
</commit_message>
<xml_diff>
--- a/Τranslations/test1_es.xlsx
+++ b/Τranslations/test1_es.xlsx
@@ -258,7 +258,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -317,12 +317,22 @@
           <t>modified</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>fi</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>se</t>
+        </is>
+      </c>
+      <c r="M1" s="0" t="inlineStr">
         <is>
           <t>es</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" s="0" t="inlineStr">
         <is>
           <t>he_IL</t>
         </is>
@@ -334,33 +344,27 @@
           <t>test</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>test 1</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>test 1 fr</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>τεστ</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="H2" s="0" t="inlineStr"/>
+      <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>δοκιμασία</t>
+        </is>
+      </c>
+      <c r="J2" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="M2" s="0" t="inlineStr">
         <is>
           <t>examen</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
+      <c r="N2" s="0" t="inlineStr">
+        <is>
+          <t>בדיקה</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -368,15 +372,31 @@
           <t>example</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr">
+      <c r="H3" s="0" t="inlineStr">
+        <is>
+          <t>test 1 fr</t>
+        </is>
+      </c>
+      <c r="I3" s="0" t="inlineStr">
+        <is>
+          <t>παράδειγμα</t>
+        </is>
+      </c>
+      <c r="J3" s="0" t="inlineStr">
+        <is>
+          <t>2023-11-09</t>
+        </is>
+      </c>
+      <c r="M3" s="0" t="inlineStr">
         <is>
           <t>ejemplo</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr"/>
+      <c r="N3" s="0" t="inlineStr">
+        <is>
+          <t>דוגמא</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -384,15 +404,31 @@
           <t>fish</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
+      <c r="H4" s="0" t="inlineStr">
+        <is>
+          <t>test 1 fr</t>
+        </is>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>ψάρι</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="inlineStr">
+        <is>
+          <t>2023-11-09</t>
+        </is>
+      </c>
+      <c r="M4" s="0" t="inlineStr">
         <is>
           <t>pez</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr"/>
+      <c r="N4" s="0" t="inlineStr">
+        <is>
+          <t>דג</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Translate newdir/test.xlsx in es [Manual Sync]
100% translated source file: 'newdir/test.xlsx'
on 'es'.
</commit_message>
<xml_diff>
--- a/Τranslations/test1_es.xlsx
+++ b/Τranslations/test1_es.xlsx
@@ -364,7 +364,7 @@
           <t>test</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>
@@ -416,7 +416,7 @@
           <t>test</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>
@@ -468,7 +468,7 @@
           <t>test</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>

</xml_diff>